<commit_message>
THis is my project
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -14,8 +14,8 @@
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" r:id="rId1"/>
-    <sheet name="ListofSurgeries" r:id="rId8" sheetId="79"/>
-    <sheet name="DoctorsDetails" r:id="rId7" sheetId="80"/>
+    <sheet name="DoctorsDetails" r:id="rId7" sheetId="86"/>
+    <sheet name="ListofSurgeries" r:id="rId8" sheetId="87"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="66">
   <si>
     <t>City</t>
   </si>
@@ -226,13 +226,173 @@
 ₹300 Consultation fee at clinic
 99% 49 Patient Stories</t>
   </si>
+  <si>
+    <t>Dr. Shilpi Gupta
+Dentist
+7 years experience overall
+Shenoy Nagar,Chennai  Forever32 Dental Care &amp; Implant Center
+₹200 Consultation fee at clinic
+100% 3 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. Kamakshi V
+Dentist
+16 years experience overall
+Perungudi,Chennai  Lumident Multispeciality Dental Centre
+₹200 Consultation fee at clinic
+100% 123 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. M. Suresh
+Dentist
+12 years experience overall
+Perumbakkam,Chennai  M.S Multi Speciality Dental Clinic
+₹100 Consultation fee at clinic
+99% 359 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. Roshan Rayen
+Dentist
+24 years experience overall
+Nungambakkam,Chennai  Rayen Dental Care Center + 1 more
+₹500 Consultation fee at clinic
+98% 216 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. Deepak Raj
+Dentist
+15 years experience overall
+Kolathur,Chennai  Raj Implant and Orthodontic Center
+₹200 Consultation fee at clinic
+99% 120 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. E. Sarath Chandar
+Dentist
+29 years experience overall
+Thiruvanmiyur,Chennai  Sarath Dental Clinic
+₹400 Consultation fee at clinic
+99% 226 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. Udhayaraja
+Dentist
+44 years experience overall
+T Nagar,Chennai  Dr. Udhayarajas Dental &amp; Orthodontic Centre + 1 more
+₹500 Consultation fee at clinic
+99% 204 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. Pavani Thota
+Dentist
+13 years experience overall
+Nungambakkam,Chennai  Dhantham Dental Hospital International + 1 more
+₹1800 Consultation fee at clinic
+97% 25 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. Chelliah Venkatraman
+Dentist
+51 years experience overall
+Adyar,Chennai  Parasu Dental Hospital + 2 more
+₹1500 Consultation fee at clinic
+92% 30 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. Gunaseelan Rajan
+Dentist
+37 years experience overall
+Mylapore,Chennai  Rajan Dental Care
+₹1500 Consultation fee at clinic
+100% 4 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. Saket Miglani
+Dentist
+25 years experience overall
+Greams Road,Chennai  Apollo Hospital + 1 more
+₹1000 Consultation fee at clinic
+100%</t>
+  </si>
+  <si>
+    <t>Dr. Kirthiga M
+Dentist
+17 years experience overall
+Anna Nagar West,Chennai  Microsmiles + 1 more
+₹300 Consultation fee at clinic
+99% 63 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. K. Anusha Unni Nishanth
+Dentist
+19 years experience overall
+Adyar,Chennai  Smile Mantra Dental &amp; Cosmetic Clinic
+₹500 Consultation fee at clinic
+99% 61 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. Mohamed Jalal
+Dentist
+9 years experience overall
+Valasaravakkam,Chennai  Sahas Dental &amp; Orthodontic Centre
+₹300 Consultation fee at clinic
+100% 24 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. H.Sharanya
+Dentist
+5 years experience overall
+Moolakadai,Chennai  Dr. Sharan's Dental Care
+₹300 Consultation fee at clinic
+100% 227 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. V.S. Hariharan
+Dentist
+22 years experience overall
+Anna Nagar West,Chennai  Kidz N Teenz + 2 more
+₹500 Consultation fee at clinic
+99% 174 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. Subramoniam S
+Dentist
+21 years experience overall
+Porur,Chennai  Lakshmi Dental Care
+₹300 Consultation fee at clinic
+99% 246 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. Subashini
+Dentist
+19 years experience overall
+Valasaravakkam,Chennai  Dew Cosmetic Clinic
+₹200 Consultation fee at clinic
+100% 93 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. K Vimala Geetha
+Dentist
+21 years experience overall
+Adyar,Chennai  Dent Eazee Speciality Dental Centres
+₹600 Consultation fee at clinic
+95% 32 Patient Stories</t>
+  </si>
+  <si>
+    <t>Dr. Sridevi. R
+Dentist
+19 years experience overall
+Semmancheri,Chennai  The Shree's Dental Clinic
+₹500 Consultation fee at clinic
+99% 72 Patient Stories</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="47" x14ac:knownFonts="1">
+  <fonts count="84" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,6 +417,191 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -511,7 +856,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -634,6 +979,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
+    <xf numFmtId="0" fontId="47" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="77" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="79" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="81" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="82" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -993,7 +1471,53 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="42.3828125"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="138">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="139">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="139">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="139">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="139">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="139">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:A20"/>
   <sheetViews>
@@ -1001,11 +1525,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.9609375"/>
+    <col min="1" max="1" width="15.9609375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="69">
+      <c r="A1" t="s" s="140">
         <v>11</v>
       </c>
     </row>
@@ -1102,27 +1626,6 @@
     <row r="20">
       <c r="A20" t="s" s="0">
         <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="true" bestFit="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="70">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>